<commit_message>
Test case 5 added Java script issue
</commit_message>
<xml_diff>
--- a/test_data/test_cases.xlsx
+++ b/test_data/test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\powerlook_hybrid_project\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7BA5A4-0DD0-407B-96BA-E55483BF50D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2012BC6F-792F-4C1D-8980-1CEB2F885EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Test Description</t>
   </si>
@@ -114,6 +114,26 @@
   <si>
     <t>1. Checkout button should be there in cart menu.
 2. Empty cart message should be displayed.</t>
+  </si>
+  <si>
+    <t>Verify sort and filter functionality of the application</t>
+  </si>
+  <si>
+    <t>1. Navigate to url
+2. Search any product.
+3. On searched product list perform low to high sort
+4. Verify price of first two products
+5. Select Price filter.
+6. Select Size filter.
+7. Verify price and size should be in range.</t>
+  </si>
+  <si>
+    <t>Applied filters and sort order should work properly</t>
+  </si>
+  <si>
+    <t>Search Product : "Shirt"
+Price Range : "₹500.00 - ₹999.99"
+Size :" L"</t>
   </si>
 </sst>
 </file>
@@ -222,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -238,9 +258,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +542,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,8 +622,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
+    <row r="7" spans="1:4" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>